<commit_message>
Updated list of jam bands
</commit_message>
<xml_diff>
--- a/jambands.xlsx
+++ b/jambands.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21060" windowHeight="9330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21060" windowHeight="9330" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Definite Jam Bands" sheetId="2" r:id="rId2"/>
     <sheet name="Likely Jam Bands" sheetId="3" r:id="rId3"/>
+    <sheet name="All Jam Bands" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="84">
   <si>
     <t>Scott definite</t>
   </si>
@@ -248,6 +249,36 @@
   </si>
   <si>
     <t>Likely</t>
+  </si>
+  <si>
+    <t>band</t>
+  </si>
+  <si>
+    <t>jamband</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>maybe</t>
+  </si>
+  <si>
+    <t>Gregg Allman &amp;Friends</t>
+  </si>
+  <si>
+    <t>Charlie Hunter Trio</t>
+  </si>
+  <si>
+    <t>Georgia Avenue &amp; Ratdog</t>
+  </si>
+  <si>
+    <t>Dead &amp; Company</t>
+  </si>
+  <si>
+    <t>Trey Anastasio (Band)</t>
+  </si>
+  <si>
+    <t>Jimi Hendrix</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1227,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1696,4 +1729,665 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
+        <f>'Definite Jam Bands'!A2</f>
+        <v>Allman Brothers Band</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="str">
+        <f>'Definite Jam Bands'!A3</f>
+        <v>Amfibian</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="str">
+        <f>'Definite Jam Bands'!A4</f>
+        <v>Big In Japan</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="str">
+        <f>'Definite Jam Bands'!A5</f>
+        <v>Blueground Undergrass</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="str">
+        <f>'Definite Jam Bands'!A6</f>
+        <v>Blues Traveler</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="str">
+        <f>'Definite Jam Bands'!A7</f>
+        <v>Bruce Hornsby</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="str">
+        <f>'Definite Jam Bands'!A8</f>
+        <v>Blueground Undergrass</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="str">
+        <f>'Definite Jam Bands'!A9</f>
+        <v>Blues Traveler</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
+        <f>'Definite Jam Bands'!A10</f>
+        <v>Built to Spill</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <f>'Definite Jam Bands'!A11</f>
+        <v>Camper Van Beethoven</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <f>'Definite Jam Bands'!A12</f>
+        <v>Charlie Hunter</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <f>'Definite Jam Bands'!A13</f>
+        <v>Disco Biscuits</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <f>'Definite Jam Bands'!A14</f>
+        <v>Drive-By Truckers</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="str">
+        <f>'Definite Jam Bands'!A15</f>
+        <v>Ekoostic Hookah</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
+        <f>'Definite Jam Bands'!A16</f>
+        <v>Galactic</v>
+      </c>
+      <c r="B16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f>'Definite Jam Bands'!A17</f>
+        <v>God Street Wine</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="str">
+        <f>'Definite Jam Bands'!A18</f>
+        <v>Grateful Dead</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="str">
+        <f>'Definite Jam Bands'!A19</f>
+        <v>Jazz Mandolin Project</v>
+      </c>
+      <c r="B19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="str">
+        <f>'Definite Jam Bands'!A20</f>
+        <v>Jerry Garcia</v>
+      </c>
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="str">
+        <f>'Definite Jam Bands'!A21</f>
+        <v>Jerry Garcia Band</v>
+      </c>
+      <c r="B21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="str">
+        <f>'Definite Jam Bands'!A22</f>
+        <v>Keller Williams</v>
+      </c>
+      <c r="B22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="str">
+        <f>'Definite Jam Bands'!A23</f>
+        <v>Lake Trout</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="str">
+        <f>'Definite Jam Bands'!A24</f>
+        <v>Little Feat</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="str">
+        <f>'Definite Jam Bands'!A25</f>
+        <v>Medeski Martin &amp; Wood</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="str">
+        <f>'Definite Jam Bands'!A26</f>
+        <v>moe.</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="str">
+        <f>'Definite Jam Bands'!A27</f>
+        <v>O.A.R.</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="str">
+        <f>'Definite Jam Bands'!A28</f>
+        <v>Oysterhead</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="str">
+        <f>'Definite Jam Bands'!A29</f>
+        <v>Pearl Jam</v>
+      </c>
+      <c r="B29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="str">
+        <f>'Definite Jam Bands'!A30</f>
+        <v>Phil Lesh &amp; Friends</v>
+      </c>
+      <c r="B30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="str">
+        <f>'Definite Jam Bands'!A31</f>
+        <v>Phish</v>
+      </c>
+      <c r="B31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="str">
+        <f>'Definite Jam Bands'!A32</f>
+        <v>Ratdog</v>
+      </c>
+      <c r="B32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="str">
+        <f>'Definite Jam Bands'!A33</f>
+        <v>Strangefolk</v>
+      </c>
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="str">
+        <f>'Definite Jam Bands'!A34</f>
+        <v>String Cheese Incident</v>
+      </c>
+      <c r="B34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="str">
+        <f>'Definite Jam Bands'!A35</f>
+        <v>Tea Leaf Green</v>
+      </c>
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="str">
+        <f>'Definite Jam Bands'!A36</f>
+        <v>The Big Woo</v>
+      </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="str">
+        <f>'Definite Jam Bands'!A37</f>
+        <v>The Dead</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="str">
+        <f>'Definite Jam Bands'!A38</f>
+        <v>The Other Ones</v>
+      </c>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="str">
+        <f>'Definite Jam Bands'!A39</f>
+        <v>Trey Anastasio Band</v>
+      </c>
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="str">
+        <f>'Definite Jam Bands'!A40</f>
+        <v>Umphrey's McGee</v>
+      </c>
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="str">
+        <f>'Definite Jam Bands'!A41</f>
+        <v>Warren Haynes</v>
+      </c>
+      <c r="B41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="str">
+        <f>'Definite Jam Bands'!A42</f>
+        <v>Ween</v>
+      </c>
+      <c r="B42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="str">
+        <f>'Definite Jam Bands'!A43</f>
+        <v>Widespread Panic</v>
+      </c>
+      <c r="B43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="str">
+        <f>'Definite Jam Bands'!A44</f>
+        <v>Yonder Mountain String Band</v>
+      </c>
+      <c r="B44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="str">
+        <f>'Likely Jam Bands'!A2</f>
+        <v>Bela Fleck &amp; The Flecktones</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="str">
+        <f>'Likely Jam Bands'!A3</f>
+        <v>Ben Harper</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="str">
+        <f>'Likely Jam Bands'!A4</f>
+        <v>Col. Claypool's Bucket of Bernie Brains</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="str">
+        <f>'Likely Jam Bands'!A5</f>
+        <v>Dark Star Orchestra</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="str">
+        <f>'Likely Jam Bands'!A6</f>
+        <v>Dave Matthews &amp; Tim Reynolds</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="str">
+        <f>'Likely Jam Bands'!A7</f>
+        <v>Dave Matthews (solo)</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="str">
+        <f>'Likely Jam Bands'!A8</f>
+        <v>Dave Matthews Band</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="str">
+        <f>'Likely Jam Bands'!A9</f>
+        <v>GreyBoy AllStars</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="str">
+        <f>'Likely Jam Bands'!A10</f>
+        <v>Guster</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="str">
+        <f>'Likely Jam Bands'!A11</f>
+        <v>Hot Tuna</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="str">
+        <f>'Likely Jam Bands'!A12</f>
+        <v>Jimi Hendrix Experience</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="str">
+        <f>'Likely Jam Bands'!A13</f>
+        <v>John Mayer</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="str">
+        <f>'Likely Jam Bands'!A14</f>
+        <v>John Scofield</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="str">
+        <f>'Likely Jam Bands'!A15</f>
+        <v>Karl Denson's Tiny Universe</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="str">
+        <f>'Likely Jam Bands'!A16</f>
+        <v>Les Claypool's Flying Frog Brigade</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="str">
+        <f>'Likely Jam Bands'!A17</f>
+        <v>North Mississippi Allstars</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="str">
+        <f>'Likely Jam Bands'!A18</f>
+        <v>Particle</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="str">
+        <f>'Likely Jam Bands'!A19</f>
+        <v>Railroad Earth</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="str">
+        <f>'Likely Jam Bands'!A20</f>
+        <v>Robert Randolph</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="str">
+        <f>'Likely Jam Bands'!A21</f>
+        <v>The John Mayer Trio</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B70" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B71" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B72" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>